<commit_message>
Updated HTML to add tooltips, fix various bugs
Updated HTML to add tooltips, fix various bugs
</commit_message>
<xml_diff>
--- a/Study_Design/ContentMap.xlsx
+++ b/Study_Design/ContentMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Google Drive\Dev\src\SSATrust\SSATrust\Study_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C42396-4FC9-403D-B49E-874B00F7E108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CBA05C-1F66-4865-BDC4-E12F18322641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{087529C0-791B-4B2B-AE78-21E23037E87A}"/>
+    <workbookView xWindow="6600" yWindow="255" windowWidth="13755" windowHeight="10875" xr2:uid="{087529C0-791B-4B2B-AE78-21E23037E87A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
   <si>
     <t>SSA Trust Content</t>
   </si>
@@ -185,6 +185,75 @@
   </si>
   <si>
     <t>web_FB_SSA.html</t>
+  </si>
+  <si>
+    <t>protectYourself.html</t>
+  </si>
+  <si>
+    <t>amazonHP.html</t>
+  </si>
+  <si>
+    <t>irs.html</t>
+  </si>
+  <si>
+    <t>IRS_YourAccount.html</t>
+  </si>
+  <si>
+    <t>appleID.html</t>
+  </si>
+  <si>
+    <t>amazonProductPage.html</t>
+  </si>
+  <si>
+    <t>mcafee.html</t>
+  </si>
+  <si>
+    <t>getProtected.html</t>
+  </si>
+  <si>
+    <t>redcross_covidRelief.html</t>
+  </si>
+  <si>
+    <t>ssa.html</t>
+  </si>
+  <si>
+    <t>mySocialSecurity.html</t>
+  </si>
+  <si>
+    <t>amazon_maskDelivery.html</t>
+  </si>
+  <si>
+    <t>ssaFb.html</t>
+  </si>
+  <si>
+    <t>ssa_optOut.html</t>
+  </si>
+  <si>
+    <t>ssa_replacementCard.html</t>
+  </si>
+  <si>
+    <t>walmart.html</t>
+  </si>
+  <si>
+    <t>Biz+Govt</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>medicareReview</t>
+  </si>
+  <si>
+    <t>benefitsSuspension</t>
+  </si>
+  <si>
+    <t>Tooltips?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -545,31 +614,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F532D942-5667-4BB6-BD8C-895099707AD2}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -595,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -614,8 +686,14 @@
       <c r="G5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -634,8 +712,14 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -654,8 +738,14 @@
       <c r="G7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -674,8 +764,14 @@
       <c r="G8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -694,8 +790,14 @@
       <c r="G9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -714,8 +816,14 @@
       <c r="G10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -734,8 +842,14 @@
       <c r="G11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -754,8 +868,14 @@
       <c r="G12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -774,8 +894,11 @@
       <c r="G14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -794,8 +917,11 @@
       <c r="G15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -814,8 +940,11 @@
       <c r="G16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -834,8 +963,11 @@
       <c r="G17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -849,13 +981,16 @@
         <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -874,8 +1009,11 @@
       <c r="G19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -894,8 +1032,11 @@
       <c r="G20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>13</v>
       </c>
@@ -913,6 +1054,43 @@
       </c>
       <c r="G21" t="s">
         <v>47</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>